<commit_message>
Fixes off-by-one in parseSheet
</commit_message>
<xml_diff>
--- a/tests/data/test.xlsx
+++ b/tests/data/test.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/scripts/dev/ingestSheet/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E9EE2D-7353-E940-A216-D9190E51598C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DE4F0E-16AD-1043-AB5F-96142AA42A63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17340" yWindow="-21140" windowWidth="28040" windowHeight="17440" xr2:uid="{D65D61B9-F8B2-FC48-9E43-219EF1851E0F}"/>
+    <workbookView xWindow="17340" yWindow="-21140" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{D65D61B9-F8B2-FC48-9E43-219EF1851E0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>parent one</t>
   </si>
@@ -97,6 +98,9 @@
   </si>
   <si>
     <t>Date:</t>
+  </si>
+  <si>
+    <t>Some notes here. Yay</t>
   </si>
 </sst>
 </file>
@@ -454,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C761BE5C-9F43-ED49-9994-5FAAFB61254B}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -643,4 +647,149 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93101268-53D5-F748-AE17-6313211C2FC2}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18:G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>14</v>
+      </c>
+      <c r="H6">
+        <v>17</v>
+      </c>
+      <c r="I6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>16</v>
+      </c>
+      <c r="H8">
+        <v>19</v>
+      </c>
+      <c r="I8">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:G4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adds in row label to dict
</commit_message>
<xml_diff>
--- a/tests/data/test.xlsx
+++ b/tests/data/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/scripts/dev/ingestSheet/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DE4F0E-16AD-1043-AB5F-96142AA42A63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68516A00-62C7-684C-BD74-14AAB793A1BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17340" yWindow="-21140" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{D65D61B9-F8B2-FC48-9E43-219EF1851E0F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19480" activeTab="1" xr2:uid="{D65D61B9-F8B2-FC48-9E43-219EF1851E0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>parent one</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Some notes here. Yay</t>
+  </si>
+  <si>
+    <t>row number</t>
   </si>
 </sst>
 </file>
@@ -138,10 +141,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,7 +462,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="A1:XFD1048576"/>
+      <selection sqref="A1:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -471,15 +474,15 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="2"/>
       <c r="I1" t="s">
         <v>9</v>
       </c>
@@ -488,6 +491,9 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -636,7 +642,7 @@
       <c r="L8" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="1">
         <v>36354</v>
       </c>
     </row>
@@ -654,7 +660,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:G19"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -668,20 +674,23 @@
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="2"/>
       <c r="I4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Adds test for merged cell into first column
</commit_message>
<xml_diff>
--- a/tests/data/test.xlsx
+++ b/tests/data/test.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/scripts/dev/ingestSheet/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68516A00-62C7-684C-BD74-14AAB793A1BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B826DF79-35DE-A648-B6EF-B3A907051ADE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19480" activeTab="1" xr2:uid="{D65D61B9-F8B2-FC48-9E43-219EF1851E0F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" activeTab="2" xr2:uid="{D65D61B9-F8B2-FC48-9E43-219EF1851E0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="23">
   <si>
     <t>parent one</t>
   </si>
@@ -659,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93101268-53D5-F748-AE17-6313211C2FC2}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -801,4 +802,154 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FF360D-E85E-B441-BFFB-7AD3D8C39EBE}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>14</v>
+      </c>
+      <c r="H6">
+        <v>17</v>
+      </c>
+      <c r="I6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>16</v>
+      </c>
+      <c r="H8">
+        <v>19</v>
+      </c>
+      <c r="I8">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>